<commit_message>
Attack HTTP request program update
</commit_message>
<xml_diff>
--- a/python_app/malicious/data/malicious_dataset.xlsx
+++ b/python_app/malicious/data/malicious_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\self\T\python_app\malicious\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2D0DD6-1DC9-4B96-BE85-C005D43B0A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D21B81B-5C52-4B2F-812B-6A2831CFFD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F99A80F8-E9C8-43A6-8B03-42E906751625}"/>
   </bookViews>
@@ -36,39 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>method</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>url</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>headers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>body</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>payload_type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>malicious</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>notes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>GET</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -205,6 +173,42 @@
   </si>
   <si>
     <t>/register</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Change Dom element</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Headers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Body</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Payload_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Malicious</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Notes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -594,48 +598,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E22C2EC9-86DA-47D2-917C-D0AEEBCA9FA4}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="59.09765625" customWidth="1"/>
     <col min="4" max="4" width="57" customWidth="1"/>
-    <col min="5" max="5" width="31.796875" customWidth="1"/>
-    <col min="6" max="6" width="20.296875" customWidth="1"/>
+    <col min="5" max="5" width="42.5" customWidth="1"/>
+    <col min="6" max="6" width="33.296875" customWidth="1"/>
     <col min="7" max="7" width="12.296875" customWidth="1"/>
     <col min="8" max="8" width="10.796875" customWidth="1"/>
-    <col min="9" max="9" width="26.3984375" customWidth="1"/>
+    <col min="9" max="9" width="35.296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -643,25 +647,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -669,22 +673,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -692,22 +696,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -715,22 +719,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -738,25 +742,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -764,22 +771,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -787,25 +794,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
         <v>19</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -813,22 +820,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I9" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.3">
@@ -836,32 +843,33 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I10" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>